<commit_message>
finalised with abstractive summarization
</commit_message>
<xml_diff>
--- a/Powerbi_reports/arb_main_dataset.xlsx
+++ b/Powerbi_reports/arb_main_dataset.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -493,7 +493,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>wav.اتصل 1</t>
+          <t>wav.اتصل 26</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -508,22 +508,22 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>0:01:22</t>
+          <t>0:01:33</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>5127.79296875</t>
+          <t>5861</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>مهارشي</t>
+          <t>سزدفغ</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>12-11-2011</t>
+          <t>12-12-1212</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -533,7 +533,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>محايد</t>
+          <t>سالب</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -543,7 +543,219 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
+          <t>0.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>wav.اتصل 27</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Call_2.wav</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>0:01:38</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>6147</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>سزدفغ</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>12-12-1212</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>الإنكليزية</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>موجب</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>0.8571428571428571</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>0.5</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>wav.اتصل 28</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Call_3.wav</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>0:01:02</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>3885</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>سزدفغ</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>12-12-1212</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>wav.اتصل 29</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Call_4.wav</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>0:01:29</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>5622</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>سزدفغ</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>12-12-1212</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>الإنكليزية</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>سالب</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
           <t>1.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>wav.اتصل 30</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Call_5.wav</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>0:01:30</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>5640</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>سزدفغ</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>12-12-1212</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>الإنكليزية</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>سالب</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>0.0</t>
         </is>
       </c>
     </row>

</xml_diff>